<commit_message>
added observations for aez 1784
</commit_message>
<xml_diff>
--- a/data/pheno_obs_1784.xlsx
+++ b/data/pheno_obs_1784.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\UserData\projects\Courses\Course_AoM\phenomodelling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{430A69AB-A0C8-406D-B2CC-2AB851BF3BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02D38C9-FCA3-4851-B9CA-074426A9B28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D4BB851C-543F-4705-A3DB-38B4065809FE}"/>
   </bookViews>
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="88">
   <si>
     <t>ObjectId</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>DOS</t>
-  </si>
-  <si>
-    <t>DOE</t>
   </si>
   <si>
     <t>DOA</t>
@@ -299,7 +296,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -783,7 +780,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1990,7 +1987,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{328EA4A7-1B0C-458A-BB75-A6939F57B57D}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{328EA4A7-1B0C-458A-BB75-A6939F57B57D}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H78" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" outline="0" showAll="0" defaultSubtotal="0">
@@ -2888,10 +2885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F311C3-758B-4D1F-830B-0821C5915916}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,10 +2896,10 @@
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
@@ -2927,11 +2924,8 @@
       <c r="H1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2951,14 +2945,11 @@
       <c r="G2" s="4">
         <v>40466</v>
       </c>
-      <c r="H2" s="4">
-        <v>40466</v>
-      </c>
-      <c r="I2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2976,14 +2967,11 @@
         <v>40408</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="4">
-        <v>40408</v>
-      </c>
-      <c r="I3" t="b">
+      <c r="H3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3005,14 +2993,11 @@
       <c r="G4" s="4">
         <v>40778</v>
       </c>
-      <c r="H4" s="4">
-        <v>40778</v>
-      </c>
-      <c r="I4" t="b">
+      <c r="H4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3030,14 +3015,11 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4">
-        <v>40747</v>
-      </c>
-      <c r="I5" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3053,14 +3035,11 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="4">
-        <v>40977</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3078,14 +3057,11 @@
         <v>41148</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="4">
-        <v>41148</v>
-      </c>
-      <c r="I7" t="b">
+      <c r="H7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3103,14 +3079,11 @@
         <v>41141</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="4">
-        <v>41141</v>
-      </c>
-      <c r="I8" t="b">
+      <c r="H8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3130,14 +3103,11 @@
       <c r="G9" s="4">
         <v>41148</v>
       </c>
-      <c r="H9" s="4">
-        <v>41148</v>
-      </c>
-      <c r="I9" t="b">
+      <c r="H9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3157,14 +3127,11 @@
       <c r="G10" s="4">
         <v>41145</v>
       </c>
-      <c r="H10" s="4">
-        <v>41145</v>
-      </c>
-      <c r="I10" t="b">
+      <c r="H10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3184,14 +3151,11 @@
       <c r="G11" s="4">
         <v>41149</v>
       </c>
-      <c r="H11" s="4">
-        <v>41149</v>
-      </c>
-      <c r="I11" t="b">
+      <c r="H11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3211,14 +3175,11 @@
       <c r="G12" s="4">
         <v>41548</v>
       </c>
-      <c r="H12" s="4">
-        <v>41548</v>
-      </c>
-      <c r="I12" t="b">
+      <c r="H12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3234,14 +3195,11 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4">
-        <v>41398</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3259,14 +3217,11 @@
         <v>41498</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4">
-        <v>41498</v>
-      </c>
-      <c r="I14" t="b">
+      <c r="H14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3282,14 +3237,11 @@
       <c r="G15" s="4">
         <v>41520</v>
       </c>
-      <c r="H15" s="4">
-        <v>41520</v>
-      </c>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3305,14 +3257,11 @@
       <c r="G16" s="4">
         <v>41520</v>
       </c>
-      <c r="H16" s="4">
-        <v>41520</v>
-      </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3328,14 +3277,11 @@
       <c r="G17" s="4">
         <v>41520</v>
       </c>
-      <c r="H17" s="4">
-        <v>41520</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3351,14 +3297,11 @@
       <c r="G18" s="4">
         <v>41520</v>
       </c>
-      <c r="H18" s="4">
-        <v>41520</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3374,14 +3317,11 @@
       <c r="G19" s="4">
         <v>41520</v>
       </c>
-      <c r="H19" s="4">
-        <v>41520</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3397,14 +3337,11 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4">
-        <v>41374</v>
-      </c>
-      <c r="I20" t="b">
+      <c r="H20" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3424,14 +3361,11 @@
       <c r="G21" s="4">
         <v>41526</v>
       </c>
-      <c r="H21" s="4">
-        <v>41526</v>
-      </c>
-      <c r="I21" t="b">
+      <c r="H21" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3447,14 +3381,11 @@
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4">
-        <v>41367</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3470,14 +3401,11 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4">
-        <v>41745</v>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -3493,14 +3421,11 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="4">
-        <v>41741</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -3518,14 +3443,11 @@
       <c r="G25" s="4">
         <v>41881</v>
       </c>
-      <c r="H25" s="4">
-        <v>41881</v>
-      </c>
-      <c r="I25" t="b">
+      <c r="H25" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -3543,14 +3465,11 @@
       <c r="G26" s="4">
         <v>41881</v>
       </c>
-      <c r="H26" s="4">
-        <v>41881</v>
-      </c>
-      <c r="I26" t="b">
+      <c r="H26" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -3566,14 +3485,11 @@
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="4">
-        <v>41740</v>
-      </c>
-      <c r="I27" t="b">
+      <c r="H27" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3591,14 +3507,11 @@
       <c r="G28" s="4">
         <v>41871</v>
       </c>
-      <c r="H28" s="4">
-        <v>41871</v>
-      </c>
-      <c r="I28" t="b">
+      <c r="H28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -3614,14 +3527,11 @@
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="4">
-        <v>41740</v>
-      </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -3637,14 +3547,11 @@
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="4">
-        <v>42101</v>
-      </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -3660,14 +3567,11 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
-      <c r="H31" s="4">
-        <v>42095</v>
-      </c>
-      <c r="I31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -3683,14 +3587,11 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
-      <c r="H32" s="4">
-        <v>42103</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -3706,14 +3607,11 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="4">
-        <v>42104</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -3729,14 +3627,11 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
-      <c r="H34" s="4">
-        <v>42103</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -3754,14 +3649,11 @@
       <c r="G35" s="4">
         <v>42591</v>
       </c>
-      <c r="H35" s="4">
-        <v>42591</v>
-      </c>
-      <c r="I35" t="b">
+      <c r="H35" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -3779,14 +3671,11 @@
       <c r="G36" s="4">
         <v>42621</v>
       </c>
-      <c r="H36" s="4">
-        <v>42621</v>
-      </c>
-      <c r="I36" t="b">
+      <c r="H36" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -3804,14 +3693,11 @@
         <v>42604</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="4">
-        <v>42604</v>
-      </c>
-      <c r="I37" t="b">
+      <c r="H37" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -3829,14 +3715,11 @@
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
-      <c r="H38" s="4">
-        <v>42559</v>
-      </c>
-      <c r="I38" t="b">
+      <c r="H38" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -3852,14 +3735,11 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
-      <c r="H39" s="4">
-        <v>42492</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -3879,14 +3759,11 @@
       <c r="G40" s="4">
         <v>42560</v>
       </c>
-      <c r="H40" s="4">
-        <v>42560</v>
-      </c>
-      <c r="I40" t="b">
+      <c r="H40" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -3908,14 +3785,11 @@
       <c r="G41" s="4">
         <v>42613</v>
       </c>
-      <c r="H41" s="4">
-        <v>42613</v>
-      </c>
-      <c r="I41" t="b">
+      <c r="H41" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -3931,14 +3805,11 @@
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
-      <c r="H42" s="4">
-        <v>42447</v>
-      </c>
-      <c r="I42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -3956,14 +3827,11 @@
         <v>42591</v>
       </c>
       <c r="G43" s="4"/>
-      <c r="H43" s="4">
-        <v>42591</v>
-      </c>
-      <c r="I43" t="b">
+      <c r="H43" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -3981,14 +3849,11 @@
         <v>42591</v>
       </c>
       <c r="G44" s="4"/>
-      <c r="H44" s="4">
-        <v>42591</v>
-      </c>
-      <c r="I44" t="b">
+      <c r="H44" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -4004,14 +3869,11 @@
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="4">
-        <v>42476</v>
-      </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -4029,14 +3891,11 @@
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
-      <c r="H46" s="4">
-        <v>42915</v>
-      </c>
-      <c r="I46" t="b">
+      <c r="H46" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -4054,14 +3913,11 @@
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="4">
-        <v>42915</v>
-      </c>
-      <c r="I47" t="b">
+      <c r="H47" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -4077,14 +3933,11 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
-      <c r="H48" s="4">
-        <v>42829</v>
-      </c>
-      <c r="I48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -4102,14 +3955,11 @@
         <v>42948</v>
       </c>
       <c r="G49" s="4"/>
-      <c r="H49" s="4">
-        <v>42948</v>
-      </c>
-      <c r="I49" t="b">
+      <c r="H49" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -4127,14 +3977,11 @@
         <v>42960</v>
       </c>
       <c r="G50" s="4"/>
-      <c r="H50" s="4">
-        <v>42960</v>
-      </c>
-      <c r="I50" t="b">
+      <c r="H50" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -4154,14 +4001,11 @@
       <c r="G51" s="4">
         <v>42982</v>
       </c>
-      <c r="H51" s="4">
-        <v>42982</v>
-      </c>
-      <c r="I51" t="b">
+      <c r="H51" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -4177,14 +4021,11 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
-      <c r="H52" s="4">
-        <v>42832</v>
-      </c>
-      <c r="I52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -4200,14 +4041,11 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="4">
-        <v>42832</v>
-      </c>
-      <c r="I53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -4223,14 +4061,11 @@
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="4">
-        <v>43294</v>
-      </c>
-      <c r="I54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -4246,14 +4081,11 @@
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="4">
-        <v>43294</v>
-      </c>
-      <c r="I55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -4271,14 +4103,11 @@
         <v>43334</v>
       </c>
       <c r="G56" s="4"/>
-      <c r="H56" s="4">
-        <v>43334</v>
-      </c>
-      <c r="I56" t="b">
+      <c r="H56" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -4296,14 +4125,11 @@
       <c r="G57" s="4">
         <v>43332</v>
       </c>
-      <c r="H57" s="4">
-        <v>43332</v>
-      </c>
-      <c r="I57" t="b">
+      <c r="H57" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -4321,14 +4147,11 @@
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
-      <c r="H58" s="4">
-        <v>43281</v>
-      </c>
-      <c r="I58" t="b">
+      <c r="H58" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -4346,14 +4169,11 @@
       <c r="G59" s="4">
         <v>43335</v>
       </c>
-      <c r="H59" s="4">
-        <v>43335</v>
-      </c>
-      <c r="I59" t="b">
+      <c r="H59" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -4369,14 +4189,11 @@
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="4">
-        <v>43211</v>
-      </c>
-      <c r="I60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -4396,14 +4213,11 @@
         <v>43326</v>
       </c>
       <c r="G61" s="4"/>
-      <c r="H61" s="4">
-        <v>43326</v>
-      </c>
-      <c r="I61" t="b">
+      <c r="H61" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -4425,14 +4239,11 @@
       <c r="G62" s="4">
         <v>43358</v>
       </c>
-      <c r="H62" s="4">
-        <v>43358</v>
-      </c>
-      <c r="I62" t="b">
+      <c r="H62" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -4448,14 +4259,11 @@
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
-      <c r="H63" s="4">
-        <v>43543</v>
-      </c>
-      <c r="I63" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -4471,14 +4279,11 @@
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
-      <c r="H64" s="4">
-        <v>43536</v>
-      </c>
-      <c r="I64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -4494,14 +4299,11 @@
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
-      <c r="H65" s="4">
-        <v>43557</v>
-      </c>
-      <c r="I65" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -4519,14 +4321,11 @@
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
-      <c r="H66" s="4">
-        <v>43668</v>
-      </c>
-      <c r="I66" t="b">
+      <c r="H66" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -4542,14 +4341,11 @@
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
-      <c r="H67" s="4">
-        <v>43544</v>
-      </c>
-      <c r="I67" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -4565,14 +4361,11 @@
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
-      <c r="H68" s="4">
-        <v>43544</v>
-      </c>
-      <c r="I68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -4590,14 +4383,11 @@
         <v>43701</v>
       </c>
       <c r="G69" s="4"/>
-      <c r="H69" s="4">
-        <v>43701</v>
-      </c>
-      <c r="I69" t="b">
+      <c r="H69" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -4615,14 +4405,11 @@
         <v>43698</v>
       </c>
       <c r="G70" s="4"/>
-      <c r="H70" s="4">
-        <v>43698</v>
-      </c>
-      <c r="I70" t="b">
+      <c r="H70" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -4640,14 +4427,11 @@
         <v>43701</v>
       </c>
       <c r="G71" s="4"/>
-      <c r="H71" s="4">
-        <v>43701</v>
-      </c>
-      <c r="I71" t="b">
+      <c r="H71" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -4663,14 +4447,11 @@
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
-      <c r="H72" s="4">
-        <v>43563</v>
-      </c>
-      <c r="I72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -4688,14 +4469,11 @@
         <v>44073</v>
       </c>
       <c r="G73" s="4"/>
-      <c r="H73" s="4">
-        <v>44073</v>
-      </c>
-      <c r="I73" t="b">
+      <c r="H73" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -4711,11 +4489,8 @@
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
-      <c r="H74" s="4">
-        <v>43921</v>
-      </c>
-      <c r="I74" t="b">
-        <v>1</v>
+      <c r="H74" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4728,7 +4503,7 @@
   <dimension ref="A3:H78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H77"/>
+      <selection activeCell="G77" sqref="A4:G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6372,7 +6147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA4E97C-9A78-4A77-937D-46F0F8F67899}">
   <dimension ref="A1:E138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection sqref="A1:E138"/>
     </sheetView>
   </sheetViews>

</xml_diff>